<commit_message>
Add u-boot relocation process description.
</commit_message>
<xml_diff>
--- a/u-boot/doc/U-Boot memory map.xlsx
+++ b/u-boot/doc/U-Boot memory map.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>0x00000000</t>
   </si>
@@ -136,10 +136,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>0x203FFF40</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Reserved
 (512B)</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -156,23 +152,10 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>0x02050000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy buffer</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Not Used</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>U-Boot
-(512KB)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>CONFIG_SYS_INIT_SP_ADDR</t>
   </si>
   <si>
@@ -200,6 +183,25 @@
   </si>
   <si>
     <t xml:space="preserve">0x02023400 : </t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x203FFF40</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>U-Boot
+(512KB)
+Stack &amp; GD are still in iROM.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>U-Boot
+(Actual size)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linux Kernel</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -324,12 +326,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -459,26 +461,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -504,35 +491,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -546,36 +515,78 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,41 +596,29 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,125 +838,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>97972</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>108857</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="任意多边形 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8632372" y="1621971"/>
-          <a:ext cx="1578428" cy="5072743"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 0 w 1164772"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 5354396"/>
-            <a:gd name="connsiteX1" fmla="*/ 195943 w 1164772"/>
-            <a:gd name="connsiteY1" fmla="*/ 1230086 h 5354396"/>
-            <a:gd name="connsiteX2" fmla="*/ 359229 w 1164772"/>
-            <a:gd name="connsiteY2" fmla="*/ 3559628 h 5354396"/>
-            <a:gd name="connsiteX3" fmla="*/ 707572 w 1164772"/>
-            <a:gd name="connsiteY3" fmla="*/ 5116286 h 5354396"/>
-            <a:gd name="connsiteX4" fmla="*/ 1164772 w 1164772"/>
-            <a:gd name="connsiteY4" fmla="*/ 5323114 h 5354396"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="1164772" h="5354396">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="68036" y="318407"/>
-                <a:pt x="136072" y="636815"/>
-                <a:pt x="195943" y="1230086"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="255814" y="1823357"/>
-                <a:pt x="273958" y="2911928"/>
-                <a:pt x="359229" y="3559628"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="444500" y="4207328"/>
-                <a:pt x="573315" y="4822372"/>
-                <a:pt x="707572" y="5116286"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="841829" y="5410200"/>
-                <a:pt x="1003300" y="5366657"/>
-                <a:pt x="1164772" y="5323114"/>
-              </a:cubicBezTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="C00000"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow" w="lg" len="lg"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1214923</xdr:colOff>
       <xdr:row>19</xdr:row>
@@ -1024,31 +904,84 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>337459</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1077686</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>576942</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>566057</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直接箭头连接符 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8392886" y="6727371"/>
+          <a:ext cx="1926771" cy="457201"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>158453</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>530319</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104190</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="矩形 15"/>
+        <xdr:cNvPr id="2" name="平行四边形 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5823859" y="1110343"/>
-          <a:ext cx="1458683" cy="489857"/>
+        <a:xfrm rot="1130948">
+          <a:off x="12350453" y="453926"/>
+          <a:ext cx="371866" cy="6736864"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
+        <a:prstGeom prst="parallelogram">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 0"/>
+          </a:avLst>
         </a:prstGeom>
-        <a:noFill/>
+        <a:solidFill>
+          <a:srgbClr val="F2A786">
+            <a:alpha val="20000"/>
+          </a:srgbClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1070,67 +1003,405 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="0"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>222337</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>22094</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>512674</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>97146</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="右箭头 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="17428042">
+          <a:off x="11449737" y="5428065"/>
+          <a:ext cx="1000338" cy="290337"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="F2A786">
+            <a:alpha val="60000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>87088</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="直接箭头连接符 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8153400" y="8469086"/>
+          <a:ext cx="2383971" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>925286</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>97974</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直接箭头连接符 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11288486" y="8479972"/>
+          <a:ext cx="2383971" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>337458</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="文本框 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7859486" y="8621485"/>
+          <a:ext cx="2841172" cy="1295401"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>void board_init_f(unsigned long bootflag)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>{ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>     copy_uboot_to_ram(); </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>     /* Jump to U-Boot image */ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>     uboot = (void *)CONFIG_SYS_TEXT_BASE; </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>X4412</a:t>
+            <a:t> (*uboot)(); /* Never returns Here */</a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1100">
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>} </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>794657</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>54430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="文本框 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11157857" y="8621487"/>
+          <a:ext cx="2841172" cy="1828799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>ENTRY(_main)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>ldr r9, [r9, #GD_BD] /* r9 = gd-&gt;bd */ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>sub r9, r9, #GD_SIZE /* new GD is below bd */ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>移植代码使用</a:t>
+            <a:t>adr lr, here ldr r0</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-            <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>, [r9, #GD_RELOC_OFF] /* </a:t>
+          </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1100">
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>r0 = gd-&gt;reloc_off */ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN"/>
+            <a:t>add lr, lr, r0 ldr r0, [r9, #GD_RELOCADDR] /* r0 = gd-&gt;relocaddr */ </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>    </a:t>
+            <a:t>b relocate_code </a:t>
           </a:r>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-            </a:rPr>
-            <a:t>　　　↓</a:t>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>...</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:latin typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-            <a:ea typeface="楷体" panose="02010609060101010101" pitchFamily="49" charset="-122"/>
-          </a:endParaRPr>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1450,8 +1721,8 @@
   </sheetPr>
   <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1473,33 +1744,33 @@
   <sheetData>
     <row r="1" spans="1:20" s="6" customFormat="1" ht="15.6">
       <c r="A1" s="7"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="10"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="8"/>
-      <c r="F1" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="F1" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="J1" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="Q1" s="7"/>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
     </row>
     <row r="2" spans="1:20" s="3" customFormat="1" ht="15.6">
       <c r="C2" s="3" t="s">
@@ -1522,459 +1793,549 @@
     </row>
     <row r="3" spans="1:20">
       <c r="F3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="R3" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="39" t="s">
-        <v>36</v>
+      <c r="G4" s="51" t="s">
+        <v>35</v>
       </c>
       <c r="J4" s="4"/>
-      <c r="K4" s="39" t="s">
-        <v>41</v>
+      <c r="K4" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="S4" s="20" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C5" s="37"/>
-      <c r="G5" s="32"/>
+      <c r="C5" s="27"/>
+      <c r="G5" s="31"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="32"/>
+      <c r="K5" s="49"/>
+      <c r="O5" s="12"/>
+      <c r="S5" s="21"/>
     </row>
     <row r="6" spans="1:20" ht="15.6">
-      <c r="C6" s="37"/>
-      <c r="G6" s="32"/>
+      <c r="C6" s="27"/>
+      <c r="G6" s="31"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="32"/>
+      <c r="K6" s="49"/>
+      <c r="O6" s="12"/>
+      <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C7" s="37"/>
-      <c r="G7" s="32"/>
+      <c r="C7" s="27"/>
+      <c r="G7" s="31"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="32"/>
+      <c r="K7" s="49"/>
+      <c r="O7" s="12"/>
+      <c r="S7" s="12"/>
     </row>
     <row r="8" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C8" s="37"/>
-      <c r="G8" s="32"/>
+      <c r="C8" s="27"/>
+      <c r="G8" s="31"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="31"/>
+      <c r="K8" s="49"/>
+      <c r="O8" s="12"/>
+      <c r="S8" s="12"/>
     </row>
     <row r="9" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="J9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>40</v>
-      </c>
+      <c r="G9" s="31"/>
+      <c r="K9" s="49"/>
+      <c r="O9" s="12"/>
+      <c r="S9" s="12"/>
     </row>
     <row r="10" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C10" s="38"/>
-      <c r="G10" s="32"/>
-      <c r="K10" s="13" t="s">
-        <v>38</v>
-      </c>
+      <c r="C10" s="28"/>
+      <c r="G10" s="31"/>
+      <c r="K10" s="49"/>
+      <c r="O10" s="12"/>
+      <c r="S10" s="12"/>
     </row>
     <row r="11" spans="1:20" ht="15.6">
-      <c r="C11" s="38"/>
-      <c r="G11" s="32"/>
+      <c r="C11" s="28"/>
+      <c r="G11" s="31"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="14"/>
+      <c r="K11" s="49"/>
+      <c r="O11" s="12"/>
+      <c r="S11" s="12"/>
     </row>
     <row r="12" spans="1:20" ht="15.6">
-      <c r="C12" s="38"/>
-      <c r="G12" s="32"/>
+      <c r="C12" s="28"/>
+      <c r="G12" s="31"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="14"/>
+      <c r="K12" s="49"/>
+      <c r="O12" s="12"/>
+      <c r="S12" s="12"/>
     </row>
     <row r="13" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="K13" s="14"/>
+      <c r="G13" s="31"/>
+      <c r="K13" s="49"/>
+      <c r="O13" s="12"/>
+      <c r="S13" s="12"/>
     </row>
     <row r="14" spans="1:20" ht="14.4" customHeight="1">
-      <c r="C14" s="42"/>
+      <c r="C14" s="30"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="32"/>
-      <c r="K14" s="14"/>
+      <c r="G14" s="31"/>
+      <c r="K14" s="49"/>
+      <c r="O14" s="12"/>
+      <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:20" ht="14.4" customHeight="1">
       <c r="B15" s="2"/>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="31" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="32"/>
+      <c r="G15" s="31"/>
       <c r="J15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="K15" s="50"/>
+      <c r="O15" s="12"/>
+      <c r="S15" s="12"/>
     </row>
     <row r="16" spans="1:20" ht="14.4" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="32"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="32"/>
-      <c r="K16" s="43" t="s">
+      <c r="G16" s="31"/>
+      <c r="K16" s="46" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C17" s="25" t="s">
+      <c r="O16" s="12"/>
+      <c r="S16" s="12"/>
+    </row>
+    <row r="17" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C17" s="20" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="32"/>
+      <c r="G17" s="31"/>
       <c r="J17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="44"/>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="C18" s="26"/>
-      <c r="G18" s="32"/>
-      <c r="K18" s="22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C19" s="26"/>
-      <c r="G19" s="32"/>
-      <c r="K19" s="23"/>
-    </row>
-    <row r="20" spans="2:15">
-      <c r="C20" s="26"/>
+        <v>47</v>
+      </c>
+      <c r="K17" s="47"/>
+      <c r="O17" s="12"/>
+      <c r="S17" s="12"/>
+    </row>
+    <row r="18" spans="2:19">
+      <c r="C18" s="21"/>
+      <c r="G18" s="31"/>
+      <c r="K18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="12"/>
+      <c r="S18" s="12"/>
+    </row>
+    <row r="19" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C19" s="21"/>
+      <c r="G19" s="31"/>
+      <c r="K19" s="40"/>
+      <c r="O19" s="12"/>
+      <c r="S19" s="12"/>
+    </row>
+    <row r="20" spans="2:19">
+      <c r="C20" s="21"/>
       <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="39"/>
       <c r="J20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="24"/>
+      <c r="K20" s="17"/>
       <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C21" s="26"/>
-      <c r="G21" s="19" t="s">
+      <c r="O20" s="12"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="12"/>
+    </row>
+    <row r="21" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C21" s="21"/>
+      <c r="G21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="13" t="s">
         <v>5</v>
       </c>
       <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C22" s="26"/>
-      <c r="G22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="O21" s="12"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="12"/>
+    </row>
+    <row r="22" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C22" s="21"/>
+      <c r="G22" s="14"/>
+      <c r="K22" s="14"/>
       <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C23" s="26"/>
-      <c r="G23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="O22" s="12"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="12"/>
+    </row>
+    <row r="23" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C23" s="21"/>
+      <c r="G23" s="14"/>
+      <c r="K23" s="14"/>
       <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C24" s="26"/>
-      <c r="G24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="O23" s="12"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="12"/>
+    </row>
+    <row r="24" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C24" s="21"/>
+      <c r="G24" s="14"/>
+      <c r="K24" s="14"/>
       <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C25" s="26"/>
-      <c r="G25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="O24" s="12"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="12"/>
+    </row>
+    <row r="25" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C25" s="21"/>
+      <c r="G25" s="14"/>
+      <c r="K25" s="14"/>
       <c r="N25" s="2"/>
-    </row>
-    <row r="26" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C26" s="26"/>
-      <c r="G26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="O25" s="12"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="12"/>
+    </row>
+    <row r="26" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C26" s="21"/>
+      <c r="G26" s="14"/>
+      <c r="K26" s="14"/>
       <c r="N26" s="2"/>
-    </row>
-    <row r="27" spans="2:15">
-      <c r="C27" s="26"/>
-      <c r="G27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="O26" s="12"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="12"/>
+    </row>
+    <row r="27" spans="2:19">
+      <c r="C27" s="21"/>
+      <c r="G27" s="14"/>
+      <c r="K27" s="14"/>
       <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="2:15">
+      <c r="O27" s="12"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="12"/>
+    </row>
+    <row r="28" spans="2:19">
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="21"/>
       <c r="F28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="21"/>
+      <c r="G28" s="15"/>
       <c r="J28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="21"/>
+      <c r="K28" s="15"/>
       <c r="N28" s="2"/>
       <c r="O28" s="5"/>
-    </row>
-    <row r="29" spans="2:15">
+      <c r="R28" s="2"/>
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="2:19">
       <c r="B29" s="2"/>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="13" t="s">
         <v>3</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="12"/>
+    </row>
+    <row r="30" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="K30" s="14"/>
       <c r="N30" s="2"/>
       <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="2:15" ht="14.4" customHeight="1">
-      <c r="C31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="12"/>
+    </row>
+    <row r="31" spans="2:19" ht="14.4" customHeight="1">
+      <c r="C31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="K31" s="14"/>
       <c r="N31" s="2"/>
       <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="2:15">
-      <c r="C32" s="20"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="12"/>
+    </row>
+    <row r="32" spans="2:19">
+      <c r="C32" s="14"/>
       <c r="F32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="21"/>
+      <c r="G32" s="15"/>
       <c r="J32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="21"/>
+      <c r="K32" s="15"/>
       <c r="N32" s="2"/>
       <c r="O32" s="5"/>
-    </row>
-    <row r="33" spans="1:15" ht="14.4" customHeight="1">
-      <c r="C33" s="20"/>
-      <c r="G33" s="22" t="s">
+      <c r="R32" s="2"/>
+      <c r="S32" s="12"/>
+    </row>
+    <row r="33" spans="1:19" ht="14.4" customHeight="1">
+      <c r="C33" s="14"/>
+      <c r="G33" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K33" s="22" t="s">
+      <c r="K33" s="16" t="s">
         <v>13</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="5"/>
-    </row>
-    <row r="34" spans="1:15" ht="14.4" customHeight="1">
-      <c r="C34" s="20"/>
-      <c r="G34" s="23"/>
-      <c r="K34" s="23"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="12"/>
+    </row>
+    <row r="34" spans="1:19" ht="14.4" customHeight="1">
+      <c r="C34" s="14"/>
+      <c r="G34" s="40"/>
+      <c r="K34" s="40"/>
       <c r="N34" s="2" t="s">
         <v>25</v>
       </c>
       <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="C35" s="20"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="12"/>
+    </row>
+    <row r="35" spans="1:19" ht="14.4" customHeight="1">
+      <c r="C35" s="14"/>
       <c r="F35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="24"/>
+      <c r="G35" s="17"/>
       <c r="J35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="24"/>
+      <c r="K35" s="17"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="O35" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="R35" s="2"/>
+      <c r="S35" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="G36" s="22" t="s">
+      <c r="C36" s="15"/>
+      <c r="G36" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="K36" s="22" t="s">
+      <c r="K36" s="16" t="s">
         <v>14</v>
       </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="26"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="O36" s="21"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="24"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="B37" s="2"/>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="24"/>
+      <c r="G37" s="17"/>
       <c r="J37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K37" s="24"/>
+      <c r="K37" s="17"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="26"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="O37" s="21"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="24"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="B38" s="2"/>
-      <c r="C38" s="20"/>
-      <c r="G38" s="22" t="s">
+      <c r="C38" s="14"/>
+      <c r="G38" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K38" s="22" t="s">
+      <c r="K38" s="16" t="s">
         <v>32</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O38" s="27"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="C39" s="20"/>
+      <c r="O38" s="22"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="24"/>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="C39" s="14"/>
       <c r="F39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="31"/>
+      <c r="G39" s="39"/>
       <c r="J39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K39" s="31"/>
+      <c r="K39" s="39"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="28"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="O39" s="33"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="24"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="G40" s="16" t="s">
+      <c r="C40" s="15"/>
+      <c r="G40" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="K40" s="16" t="s">
+      <c r="K40" s="36" t="s">
         <v>19</v>
       </c>
       <c r="N40" s="2"/>
-      <c r="O40" s="29"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="O40" s="34"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="24"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="B41" s="2"/>
-      <c r="C41" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G41" s="17"/>
-      <c r="K41" s="17"/>
+      <c r="C41" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="37"/>
+      <c r="K41" s="37"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="29"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="O41" s="34"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="24"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="B42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="24"/>
+      <c r="C42" s="17"/>
       <c r="F42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G42" s="18"/>
+      <c r="G42" s="38"/>
       <c r="J42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K42" s="18"/>
+      <c r="K42" s="38"/>
       <c r="N42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O42" s="30"/>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="46"/>
-      <c r="B46" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="46" t="s">
+      <c r="O42" s="35"/>
+      <c r="R42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S42" s="25"/>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" s="9"/>
+      <c r="B46" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" s="9"/>
+      <c r="B48" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" s="46"/>
-      <c r="B47" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="46" t="s">
+      <c r="C48" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="A48" s="46"/>
-      <c r="B48" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="65" ht="14.4" customHeight="1"/>
     <row r="77" ht="14.4" customHeight="1"/>
     <row r="85" ht="14.4" customHeight="1"/>
     <row r="89" ht="14.4" customHeight="1"/>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="K4:K15"/>
+    <mergeCell ref="G4:G20"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="G38:G39"/>
     <mergeCell ref="G40:G42"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="K10:K15"/>
-    <mergeCell ref="G4:G20"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="K21:K28"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="K33:K35"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="S35:S42"/>
     <mergeCell ref="C4:C8"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C28"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="C41:C42"/>
     <mergeCell ref="O35:O38"/>
     <mergeCell ref="O39:O42"/>
     <mergeCell ref="K40:K42"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="G21:G28"/>
-    <mergeCell ref="K21:K28"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="K33:K35"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="K18:K20"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>